<commit_message>
Nest step test and map IRIS
</commit_message>
<xml_diff>
--- a/IrbAnalyser/event.xlsx
+++ b/IrbAnalyser/event.xlsx
@@ -1,23 +1,97 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+  <si>
+    <t>StudyId</t>
+  </si>
+  <si>
+    <t>StudySiteId</t>
+  </si>
+  <si>
+    <t>IRBAgency</t>
+  </si>
+  <si>
+    <t>IRBNumber</t>
+  </si>
+  <si>
+    <t>EventID</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>EventCreationDate</t>
+  </si>
+  <si>
+    <t>EventOutcome</t>
+  </si>
+  <si>
+    <t>TaskCompletionDate</t>
+  </si>
+  <si>
+    <t>EventCompletionDate</t>
+  </si>
+  <si>
+    <t>BRANY</t>
+  </si>
+  <si>
+    <t>Einstein</t>
+  </si>
+  <si>
+    <t>"654654"</t>
+  </si>
+  <si>
+    <t>"4564654"</t>
+  </si>
+  <si>
+    <t>"632132"</t>
+  </si>
+  <si>
+    <t>"64654"</t>
+  </si>
+  <si>
+    <t>"12345"</t>
+  </si>
+  <si>
+    <t>"123465498"</t>
+  </si>
+  <si>
+    <t>"IRBAmendment"</t>
+  </si>
+  <si>
+    <t>2015-03-12T08:22:12</t>
+  </si>
+  <si>
+    <t>2015-04-12T08:22:12</t>
+  </si>
+  <si>
+    <t>Sitename</t>
+  </si>
+  <si>
+    <t>Einstein-Montefiore</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,7 +127,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -343,36 +422,142 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="5" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>